<commit_message>
update website views and logics
</commit_message>
<xml_diff>
--- a/src/assets/excel/Record.xlsx
+++ b/src/assets/excel/Record.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="331">
   <si>
     <t>Name</t>
   </si>
@@ -1006,7 +1006,7 @@
     <t>Villasoto, Lara Kamelle C.</t>
   </si>
   <si>
-    <t>jhgjhgj l. jghghgh</t>
+    <t>Gamil, Mon Albert L.</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1014,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1061,6 +1061,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1091,7 +1097,7 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -1121,7 +1127,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
@@ -1441,10 +1447,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="26.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="5.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="34.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="19.005" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="14" width="13.862142857142858" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="14" width="16.576428571428572" customWidth="1" bestFit="1"/>
@@ -4023,7 +4029,7 @@
       <c r="G143" s="4"/>
       <c r="H143" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="19.5">
       <c r="A144" s="5" t="s">
         <v>294</v>
       </c>
@@ -4041,7 +4047,7 @@
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="19.5">
       <c r="A145" s="5" t="s">
         <v>296</v>
       </c>
@@ -4059,7 +4065,7 @@
       <c r="G145" s="4"/>
       <c r="H145" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="19.5">
       <c r="A146" s="5" t="s">
         <v>298</v>
       </c>
@@ -4077,7 +4083,7 @@
       <c r="G146" s="4"/>
       <c r="H146" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="19.5">
       <c r="A147" s="5" t="s">
         <v>300</v>
       </c>
@@ -4095,7 +4101,7 @@
       <c r="G147" s="4"/>
       <c r="H147" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5">
       <c r="A148" s="5" t="s">
         <v>302</v>
       </c>
@@ -4113,7 +4119,7 @@
       <c r="G148" s="4"/>
       <c r="H148" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="19.5">
       <c r="A149" s="5" t="s">
         <v>304</v>
       </c>
@@ -4131,7 +4137,7 @@
       <c r="G149" s="4"/>
       <c r="H149" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="19.5">
       <c r="A150" s="5" t="s">
         <v>306</v>
       </c>
@@ -4149,7 +4155,7 @@
       <c r="G150" s="4"/>
       <c r="H150" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="19.5">
       <c r="A151" s="5" t="s">
         <v>308</v>
       </c>
@@ -4167,7 +4173,7 @@
       <c r="G151" s="4"/>
       <c r="H151" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="19.5">
       <c r="A152" s="5" t="s">
         <v>310</v>
       </c>
@@ -4185,7 +4191,7 @@
       <c r="G152" s="4"/>
       <c r="H152" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5">
       <c r="A153" s="5" t="s">
         <v>312</v>
       </c>
@@ -4203,7 +4209,7 @@
       <c r="G153" s="4"/>
       <c r="H153" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="19.5">
       <c r="A154" s="5" t="s">
         <v>314</v>
       </c>
@@ -4221,7 +4227,7 @@
       <c r="G154" s="4"/>
       <c r="H154" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="19.5">
       <c r="A155" s="5" t="s">
         <v>316</v>
       </c>
@@ -4239,7 +4245,7 @@
       <c r="G155" s="4"/>
       <c r="H155" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="19.5">
       <c r="A156" s="5" t="s">
         <v>318</v>
       </c>
@@ -4257,7 +4263,7 @@
       <c r="G156" s="4"/>
       <c r="H156" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5">
       <c r="A157" s="5" t="s">
         <v>320</v>
       </c>
@@ -4275,7 +4281,7 @@
       <c r="G157" s="4"/>
       <c r="H157" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5">
       <c r="A158" s="5" t="s">
         <v>322</v>
       </c>
@@ -4293,7 +4299,7 @@
       <c r="G158" s="4"/>
       <c r="H158" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5">
       <c r="A159" s="5" t="s">
         <v>324</v>
       </c>
@@ -4311,7 +4317,7 @@
       <c r="G159" s="4"/>
       <c r="H159" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5">
       <c r="A160" s="5" t="s">
         <v>326</v>
       </c>
@@ -4329,7 +4335,7 @@
       <c r="G160" s="4"/>
       <c r="H160" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5">
       <c r="A161" s="5" t="s">
         <v>328</v>
       </c>
@@ -4347,19 +4353,25 @@
       <c r="G161" s="4"/>
       <c r="H161" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
-      <c r="A162" s="11"/>
-      <c r="B162" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="19.5">
+      <c r="A162" s="5">
+        <v>161</v>
+      </c>
+      <c r="B162" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="C162" s="4"/>
-      <c r="D162" s="4"/>
+      <c r="C162" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E162" s="4"/>
       <c r="F162" s="4"/>
       <c r="G162" s="4"/>
       <c r="H162" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="19.5">
       <c r="A163" s="11"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
@@ -4369,7 +4381,7 @@
       <c r="G163" s="4"/>
       <c r="H163" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5">
       <c r="A164" s="11"/>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
@@ -4379,7 +4391,7 @@
       <c r="G164" s="4"/>
       <c r="H164" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="19.5">
       <c r="A165" s="11"/>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
@@ -4389,7 +4401,7 @@
       <c r="G165" s="4"/>
       <c r="H165" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="19.5">
       <c r="A166" s="11"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
@@ -4399,7 +4411,7 @@
       <c r="G166" s="4"/>
       <c r="H166" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="19.5">
       <c r="A167" s="11"/>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
@@ -4409,7 +4421,7 @@
       <c r="G167" s="4"/>
       <c r="H167" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="19.5">
       <c r="A168" s="11"/>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
@@ -4419,7 +4431,7 @@
       <c r="G168" s="4"/>
       <c r="H168" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="19.5">
       <c r="A169" s="11"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
@@ -4429,7 +4441,7 @@
       <c r="G169" s="4"/>
       <c r="H169" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="19.5">
       <c r="A170" s="11"/>
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
@@ -4439,7 +4451,7 @@
       <c r="G170" s="4"/>
       <c r="H170" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="19.5">
       <c r="A171" s="12"/>
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
@@ -4449,7 +4461,7 @@
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="19.5">
       <c r="A172" s="12"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
@@ -4459,7 +4471,7 @@
       <c r="G172" s="4"/>
       <c r="H172" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="19.5">
       <c r="A173" s="12"/>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
@@ -4469,7 +4481,7 @@
       <c r="G173" s="4"/>
       <c r="H173" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="19.5">
       <c r="A174" s="12"/>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
@@ -4479,7 +4491,7 @@
       <c r="G174" s="4"/>
       <c r="H174" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="19.5">
       <c r="A175" s="12"/>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
@@ -4489,7 +4501,7 @@
       <c r="G175" s="4"/>
       <c r="H175" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="19.5">
       <c r="A176" s="12"/>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
@@ -4499,7 +4511,7 @@
       <c r="G176" s="4"/>
       <c r="H176" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="19.5">
       <c r="A177" s="12"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>

</xml_diff>